<commit_message>
Correction des bugs, ajout du score
</commit_message>
<xml_diff>
--- a/documentation/306_Journal_travail_ArcardiaBox_ROMANENS_NOE.xlsx
+++ b/documentation/306_Journal_travail_ArcardiaBox_ROMANENS_NOE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noe/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noe/Documents/emf_pro/306/306-project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A65CF74C-7C41-C64A-AE20-F2D52F4D50E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463D25D3-F1BA-A646-9B80-07D418DA6496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>Problème</t>
   </si>
@@ -109,7 +109,28 @@
     <t>Romanens Noé</t>
   </si>
   <si>
-    <t>La semaine s'est bien passée, on a bien avancé le projet et tout roule, je suis content de ce qu'on a accompli jusqu'à maintenant.</t>
+    <t>Mise en place de l'interface d'ArcadiaBox, début du développement</t>
+  </si>
+  <si>
+    <t>Développement du premier jeu</t>
+  </si>
+  <si>
+    <t>Peaufinage du premier jeu</t>
+  </si>
+  <si>
+    <t>Mise en place propre modèle MVC, et compatibilité manette pour le jeu</t>
+  </si>
+  <si>
+    <t>Implémentation du deuxième jeu et des scores</t>
+  </si>
+  <si>
+    <t>Corrections des bugs et peaufinage</t>
+  </si>
+  <si>
+    <t>Cette semaine a été très productive, j'ai pu avancer sur de nombreux points au niveau du développement, je pense que le produit est prêt pour une première version a être démontrée au client.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La semaine s'est bien passée, je trouve que le projet a bien avancé et tout roule, je suis content de ce qu'on a accompli jusqu'à maintenant. Plusieurs schémas sont terminés, de la documentation a été vue et revue, la structure de base est mise en place et tout est fin prêt pour le début du développement de la v1 </t>
   </si>
 </sst>
 </file>
@@ -535,6 +556,46 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -543,6 +604,50 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -552,90 +657,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1145,10 +1166,10 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E21" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1165,20 +1186,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="H2" s="15"/>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -1191,13 +1212,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="41"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1207,9 +1228,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1219,11 +1240,11 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="47">
+      <c r="A6" s="23">
         <v>45992</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -1312,10 +1333,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="24"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="10" t="s">
         <v>10</v>
       </c>
@@ -1325,31 +1346,31 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18">
         <v>45999</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="18"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="18"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -1367,22 +1388,22 @@
       <c r="A24" s="17">
         <v>45999</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="18"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="18"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
@@ -1400,9 +1421,13 @@
       <c r="A28" s="17">
         <v>46000</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="C28" s="20"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="18"/>
@@ -1424,48 +1449,54 @@
       </c>
       <c r="D31" s="8">
         <f>SUM(D28:D30)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="24"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="11">
         <f>SUM(D23,D27,D31)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="A33" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="31">
+      <c r="A34" s="45">
         <v>46006</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="C34" s="20"/>
-      <c r="D34" s="7"/>
+      <c r="D34" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="18"/>
-      <c r="B35" s="21"/>
+      <c r="B35" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="C35" s="22"/>
-      <c r="D35" s="7"/>
+      <c r="D35" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="18"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="22"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
@@ -1476,16 +1507,20 @@
       </c>
       <c r="D37" s="8">
         <f>SUM(D34:D36)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
         <v>46006</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="6"/>
+      <c r="B38" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="18"/>
@@ -1507,22 +1542,30 @@
       </c>
       <c r="D41" s="8">
         <f>SUM(D38:D40)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="17">
         <v>46007</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="C42" s="20"/>
-      <c r="D42" s="6"/>
+      <c r="D42" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="18"/>
-      <c r="B43" s="21"/>
+      <c r="B43" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="C43" s="22"/>
-      <c r="D43" s="7"/>
+      <c r="D43" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="18"/>
@@ -1538,27 +1581,29 @@
       </c>
       <c r="D45" s="8">
         <f>SUM(D42:D44)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="24"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="11">
         <f>SUM(D37,D41,D45)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="28"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="30"/>
+      <c r="A47" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="37"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="18">
@@ -1654,10 +1699,10 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B60" s="24"/>
+      <c r="B60" s="34"/>
       <c r="C60" s="10" t="s">
         <v>10</v>
       </c>
@@ -1667,10 +1712,10 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="25"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="27"/>
+      <c r="A61" s="46"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="48"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="18">
@@ -1766,10 +1811,10 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="24"/>
+      <c r="B74" s="34"/>
       <c r="C74" s="10" t="s">
         <v>10</v>
       </c>
@@ -1784,57 +1829,24 @@
       </c>
       <c r="D76" s="9">
         <f>D18+D32+D46+D60+D74</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="69">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B20:C22"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B24:C26"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+  <mergeCells count="68">
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B66:C66"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A61:D61"/>
     <mergeCell ref="A52:A55"/>
@@ -1845,19 +1857,51 @@
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B24:C26"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B20:C22"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D17">
     <cfRule type="containsText" dxfId="11" priority="31" operator="containsText" text="Terminé">
@@ -1922,81 +1966,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AppVersion xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Invited_Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Owner xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Teams_Channel_Section_Location xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <TeamsChannelId xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Invited_Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <FolderType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <CultureName xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Student_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Self_Registration_Enabled xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Templates xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <LMS_Mappings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <NotebookType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Distribution_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Math_Settings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <TaxCatchAll xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" xsi:nil="true"/>
-    <SharedWithUsers xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Groupe xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Langue xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">FD = français voie bili</Langue>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100280ED870E36F6F4C976CEAC6988F82A5" ma:contentTypeVersion="37" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3169f06de23f2334ced166a676265d3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xmlns:ns3="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eab9665bb0af9cfdaba242b84d69e760" ns2:_="" ns3:_="">
     <xsd:import namespace="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
@@ -2433,10 +2402,96 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AppVersion xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Invited_Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Owner xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Teams_Channel_Section_Location xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <TeamsChannelId xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Invited_Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <FolderType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <CultureName xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Student_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Self_Registration_Enabled xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Templates xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <LMS_Mappings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <NotebookType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Distribution_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Math_Settings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <TaxCatchAll xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" xsi:nil="true"/>
+    <SharedWithUsers xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Groupe xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Langue xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">FD = français voie bili</Langue>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA445AE9-3816-4E66-9DE6-AF42B0662460}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
+    <ds:schemaRef ds:uri="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2459,20 +2514,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA445AE9-3816-4E66-9DE6-AF42B0662460}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
-    <ds:schemaRef ds:uri="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modifs journal de travail
</commit_message>
<xml_diff>
--- a/documentation/306_Journal_travail_ArcardiaBox_ROMANENS_NOE.xlsx
+++ b/documentation/306_Journal_travail_ArcardiaBox_ROMANENS_NOE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noe/Documents/emf_pro/306/306-project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1407EA5E-4723-D348-9CF7-61BE7E3C7FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA8B40F-0A73-C14B-8C8A-F32B4B99FEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>Problème</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Corrections des bugs restants que ce soit sur l'interface, les jeux, les scores, mise au propre MVC.</t>
+  </si>
+  <si>
+    <t>Pour un début de projet je trouve que j'ai bien avancé, le projet qu'on doit faire me plaît personnellement donc je pense qu'on va pouvoir faire quelque chose de très beau et "stylé". J'ai hâte de continuer ce projet, la base de l'architecture et du déroulement de projet annonce de bonne chose pour la suite</t>
+  </si>
+  <si>
+    <t>Début de l'implémentation des photos de profil (fonctionnalité en plus demandée)</t>
+  </si>
+  <si>
+    <t>Cette semaine a été productive, j'ai pu corriger pas mal de points qui dérangeaient et ça allège l'esprit de savoir que le projet est bien plus propre qu'avant tant au niveau de l'organisation du code que du visuel, ça s'annonce très bien également avec le début de l'implémentation d'une nouvelle fonctionnalité de photo de profil pour les comptes, dommage qu'on n'y ait pas pensé avant cela va rendre vraiment bien d'après moi.</t>
   </si>
 </sst>
 </file>
@@ -501,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -586,6 +595,46 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -594,8 +643,44 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -606,88 +691,8 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1196,10 +1201,10 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E47" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomRight" activeCell="A62" sqref="A62:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1216,20 +1221,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="H2" s="15"/>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -1242,13 +1247,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1258,9 +1263,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1270,13 +1275,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="48">
+      <c r="A6" s="23">
         <v>45992</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="6">
         <v>2</v>
       </c>
@@ -1383,10 +1388,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="24"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="10" t="s">
         <v>10</v>
       </c>
@@ -1396,31 +1401,33 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="38"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="A19" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18">
         <v>45999</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="18"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="18"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -1438,22 +1445,22 @@
       <c r="A24" s="17">
         <v>45999</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="18"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="18"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
@@ -1503,10 +1510,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="24"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="10" t="s">
         <v>10</v>
       </c>
@@ -1516,15 +1523,15 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="36"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="31">
+      <c r="A34" s="44">
         <v>46006</v>
       </c>
       <c r="B34" s="19" t="s">
@@ -1635,10 +1642,10 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="24"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="10" t="s">
         <v>10</v>
       </c>
@@ -1648,12 +1655,12 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="30"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="36"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="18">
@@ -1742,14 +1749,18 @@
       </c>
       <c r="C56" s="20"/>
       <c r="D56" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="18"/>
-      <c r="B57" s="21"/>
+      <c r="B57" s="21" t="s">
+        <v>34</v>
+      </c>
       <c r="C57" s="22"/>
-      <c r="D57" s="7"/>
+      <c r="D57" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="18"/>
@@ -1769,10 +1780,10 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B60" s="24"/>
+      <c r="B60" s="34"/>
       <c r="C60" s="10" t="s">
         <v>10</v>
       </c>
@@ -1782,10 +1793,12 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="25"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="27"/>
+      <c r="A61" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="45"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="46"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="18">
@@ -1881,10 +1894,10 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="24"/>
+      <c r="B74" s="34"/>
       <c r="C74" s="10" t="s">
         <v>10</v>
       </c>
@@ -1904,51 +1917,19 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B20:C22"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B24:C26"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B66:C66"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A61:D61"/>
     <mergeCell ref="A52:A55"/>
@@ -1959,19 +1940,51 @@
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B24:C26"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B20:C22"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D17">
     <cfRule type="containsText" dxfId="11" priority="31" operator="containsText" text="Terminé">
@@ -2036,81 +2049,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AppVersion xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Invited_Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Owner xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Teams_Channel_Section_Location xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <TeamsChannelId xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Invited_Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <FolderType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <CultureName xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Student_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Self_Registration_Enabled xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Templates xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <LMS_Mappings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <NotebookType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Distribution_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Math_Settings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <TaxCatchAll xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" xsi:nil="true"/>
-    <SharedWithUsers xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Groupe xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
-    <Langue xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">FD = français voie bili</Langue>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100280ED870E36F6F4C976CEAC6988F82A5" ma:contentTypeVersion="37" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3169f06de23f2334ced166a676265d3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xmlns:ns3="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eab9665bb0af9cfdaba242b84d69e760" ns2:_="" ns3:_="">
     <xsd:import namespace="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
@@ -2547,10 +2485,96 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AppVersion xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Invited_Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Owner xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Teams_Channel_Section_Location xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <TeamsChannelId xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Invited_Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <FolderType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <CultureName xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Student_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Self_Registration_Enabled xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Teachers xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Templates xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <LMS_Mappings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <NotebookType xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Distribution_Groups xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Math_Settings xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <TaxCatchAll xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5" xsi:nil="true"/>
+    <SharedWithUsers xmlns="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Groupe xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea" xsi:nil="true"/>
+    <Langue xmlns="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea">FD = français voie bili</Langue>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA445AE9-3816-4E66-9DE6-AF42B0662460}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
+    <ds:schemaRef ds:uri="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2573,20 +2597,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA445AE9-3816-4E66-9DE6-AF42B0662460}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A0F71E-9B9F-4628-8A94-D320BA80A1D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="32d4d717-cd3a-4b3d-8168-24cfd96cd6ea"/>
-    <ds:schemaRef ds:uri="5cbbe46b-cb1d-4e56-8c99-5e3dbfb293e5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>